<commit_message>
Create new models for results prdiction
</commit_message>
<xml_diff>
--- a/Emsc2404Semis.xlsx
+++ b/Emsc2404Semis.xlsx
@@ -667,17 +667,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S24" activeCellId="0" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
@@ -686,7 +686,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="1" width="4.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="15" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="29" style="1" width="2.72"/>
   </cols>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="T4" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -1343,7 +1343,7 @@
         <v>16</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="T8" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T10" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -1938,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="S15" s="2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T15" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -2108,7 +2108,7 @@
         <v>5</v>
       </c>
       <c r="S17" s="2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="T17" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -2278,7 +2278,7 @@
         <v>9</v>
       </c>
       <c r="S19" s="2" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="T19" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -2363,7 +2363,7 @@
         <v>4</v>
       </c>
       <c r="S20" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T20" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -2448,7 +2448,7 @@
         <v>15</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T21" s="3" t="b">
         <f aca="false">TRUE()</f>
@@ -2618,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="S23" s="2" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="T23" s="3" t="b">
         <f aca="false">TRUE()</f>

</xml_diff>